<commit_message>
updating real bio details
</commit_message>
<xml_diff>
--- a/_files/requirements/RealBiometrics Dependencies.xlsx
+++ b/_files/requirements/RealBiometrics Dependencies.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://pws.mindtree.com/projects/NP-087/Docs/MOSIP_Project Management/Real Biometrics/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\M1045436\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19160" windowHeight="6890"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6950"/>
   </bookViews>
   <sheets>
     <sheet name="Features" sheetId="1" r:id="rId1"/>
@@ -17,9 +17,9 @@
     <sheet name="Legends" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Features!$A$1:$N$32</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Features!$A$1:$P$32</definedName>
   </definedNames>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="163">
   <si>
     <t>Sl No.</t>
   </si>
@@ -124,9 +124,6 @@
   </si>
   <si>
     <t>16th Oct</t>
-  </si>
-  <si>
-    <t>Yashwanth</t>
   </si>
   <si>
     <t>Update UIN – Biometric Data Capture</t>
@@ -463,9 +460,6 @@
     <t>3rd Oct</t>
   </si>
   <si>
-    <t>Mukul and Taleev</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Status Comments</t>
   </si>
   <si>
@@ -515,13 +509,37 @@
   </si>
   <si>
     <t>Internal</t>
+  </si>
+  <si>
+    <t>Taleev</t>
+  </si>
+  <si>
+    <t>Dev Complete</t>
+  </si>
+  <si>
+    <t>Sprint 20</t>
+  </si>
+  <si>
+    <t>Sprint 19</t>
+  </si>
+  <si>
+    <t>TBD</t>
+  </si>
+  <si>
+    <t>Test Complete</t>
+  </si>
+  <si>
+    <t>Sprint 21</t>
+  </si>
+  <si>
+    <t>Usha</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -554,6 +572,27 @@
       <color theme="0"/>
       <name val="Cambria"/>
       <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="13">
@@ -629,7 +668,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -736,11 +775,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -748,36 +802,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -787,21 +811,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -863,15 +872,64 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="134">
+  <dxfs count="137">
     <dxf>
       <fill>
         <patternFill>
@@ -1023,6 +1081,27 @@
       <fill>
         <patternFill>
           <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2120,1723 +2199,1936 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O32"/>
+  <dimension ref="A1:Q33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="J25" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="topRight" activeCell="E1" sqref="E1"/>
-      <selection pane="bottomRight" activeCell="J28" sqref="J28"/>
+      <selection pane="bottomRight" activeCell="N43" sqref="N43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="14.1"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.5703125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="8.7109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="25.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="5.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.90625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="22.54296875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="8.7265625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="25.7265625" style="1" customWidth="1"/>
     <col min="7" max="7" width="15" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.28515625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="55.85546875" style="1" customWidth="1"/>
-    <col min="10" max="10" width="13.7109375" style="2" customWidth="1"/>
-    <col min="11" max="11" width="14.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="49.42578125" style="1" customWidth="1"/>
-    <col min="15" max="16384" width="8.7109375" style="1"/>
+    <col min="8" max="8" width="11.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="38" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.7265625" style="2" customWidth="1"/>
+    <col min="11" max="11" width="10.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="14.7265625" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.1796875" style="2" customWidth="1"/>
+    <col min="15" max="15" width="11.453125" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="59.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="3" customFormat="1" ht="27.6" customHeight="1">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:17" s="3" customFormat="1" ht="27.65" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="E1" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="F1" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="G1" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="14" t="s">
+      <c r="H1" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="14" t="s">
+      <c r="I1" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="15" t="s">
+      <c r="J1" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="15" t="s">
+      <c r="K1" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" s="27" t="s">
+        <v>156</v>
+      </c>
+      <c r="M1" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="15" t="s">
+      <c r="N1" s="27" t="s">
+        <v>160</v>
+      </c>
+      <c r="O1" s="27" t="s">
+        <v>12</v>
+      </c>
+      <c r="P1" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q1" s="6"/>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A2" s="32">
+        <v>1</v>
+      </c>
+      <c r="B2" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="33" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="34" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="36" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" s="35" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2" s="36" t="s">
+        <v>20</v>
+      </c>
+      <c r="K2" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="L2" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="M2" s="32">
+        <v>0.5</v>
+      </c>
+      <c r="N2" s="32" t="s">
+        <v>158</v>
+      </c>
+      <c r="O2" s="37" t="s">
+        <v>21</v>
+      </c>
+      <c r="P2" s="33" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A3" s="32">
+        <v>2</v>
+      </c>
+      <c r="B3" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="33" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="38" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="35"/>
+      <c r="G3" s="35"/>
+      <c r="H3" s="36" t="s">
+        <v>18</v>
+      </c>
+      <c r="I3" s="33"/>
+      <c r="J3" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="K3" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="L3" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="M3" s="32">
+        <v>3</v>
+      </c>
+      <c r="N3" s="32" t="s">
+        <v>158</v>
+      </c>
+      <c r="O3" s="37" t="s">
+        <v>21</v>
+      </c>
+      <c r="P3" s="33" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A4" s="32">
+        <v>3</v>
+      </c>
+      <c r="B4" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="33" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="34" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="G4" s="35"/>
+      <c r="H4" s="36" t="s">
+        <v>27</v>
+      </c>
+      <c r="I4" s="33" t="s">
+        <v>28</v>
+      </c>
+      <c r="J4" s="39" t="s">
+        <v>29</v>
+      </c>
+      <c r="K4" s="32">
+        <v>2</v>
+      </c>
+      <c r="L4" s="32" t="s">
+        <v>157</v>
+      </c>
+      <c r="M4" s="32">
+        <v>2</v>
+      </c>
+      <c r="N4" s="32" t="s">
+        <v>161</v>
+      </c>
+      <c r="O4" s="32" t="s">
+        <v>155</v>
+      </c>
+      <c r="P4" s="33"/>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A5" s="32">
+        <v>4</v>
+      </c>
+      <c r="B5" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="33" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" s="34" t="s">
+        <v>31</v>
+      </c>
+      <c r="E5" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="35"/>
+      <c r="G5" s="35"/>
+      <c r="H5" s="36" t="s">
+        <v>18</v>
+      </c>
+      <c r="I5" s="35" t="s">
+        <v>32</v>
+      </c>
+      <c r="J5" s="36" t="s">
+        <v>20</v>
+      </c>
+      <c r="K5" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="L5" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="M5" s="32">
+        <v>3</v>
+      </c>
+      <c r="N5" s="32" t="s">
+        <v>158</v>
+      </c>
+      <c r="O5" s="37" t="s">
+        <v>21</v>
+      </c>
+      <c r="P5" s="33" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A6" s="32">
+        <v>5</v>
+      </c>
+      <c r="B6" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="33" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" s="38" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" s="35"/>
+      <c r="G6" s="35"/>
+      <c r="H6" s="36" t="s">
+        <v>18</v>
+      </c>
+      <c r="I6" s="33"/>
+      <c r="J6" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="K6" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="L6" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="M6" s="32">
+        <v>2</v>
+      </c>
+      <c r="N6" s="32" t="s">
+        <v>158</v>
+      </c>
+      <c r="O6" s="37" t="s">
+        <v>162</v>
+      </c>
+      <c r="P6" s="33" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A7" s="32">
+        <v>6</v>
+      </c>
+      <c r="B7" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7" s="38" t="s">
+        <v>35</v>
+      </c>
+      <c r="E7" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" s="35" t="s">
+        <v>36</v>
+      </c>
+      <c r="G7" s="35"/>
+      <c r="H7" s="36" t="s">
+        <v>37</v>
+      </c>
+      <c r="I7" s="33" t="s">
+        <v>28</v>
+      </c>
+      <c r="J7" s="39" t="s">
+        <v>29</v>
+      </c>
+      <c r="K7" s="32">
+        <v>3</v>
+      </c>
+      <c r="L7" s="32" t="s">
+        <v>157</v>
+      </c>
+      <c r="M7" s="32">
+        <v>2</v>
+      </c>
+      <c r="N7" s="32" t="s">
+        <v>161</v>
+      </c>
+      <c r="O7" s="32" t="s">
+        <v>155</v>
+      </c>
+      <c r="P7" s="33" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A8" s="32">
+        <v>7</v>
+      </c>
+      <c r="B8" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="33" t="s">
+        <v>39</v>
+      </c>
+      <c r="D8" s="38" t="s">
+        <v>40</v>
+      </c>
+      <c r="E8" s="32" t="s">
+        <v>41</v>
+      </c>
+      <c r="F8" s="35" t="s">
+        <v>42</v>
+      </c>
+      <c r="G8" s="35" t="s">
+        <v>43</v>
+      </c>
+      <c r="H8" s="36" t="s">
+        <v>37</v>
+      </c>
+      <c r="I8" s="33" t="s">
+        <v>44</v>
+      </c>
+      <c r="J8" s="40" t="s">
+        <v>45</v>
+      </c>
+      <c r="K8" s="32">
+        <v>3</v>
+      </c>
+      <c r="L8" s="32" t="s">
+        <v>158</v>
+      </c>
+      <c r="M8" s="32">
+        <v>1</v>
+      </c>
+      <c r="N8" s="32" t="s">
+        <v>157</v>
+      </c>
+      <c r="O8" s="32" t="s">
+        <v>155</v>
+      </c>
+      <c r="P8" s="33"/>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A9" s="32">
+        <v>8</v>
+      </c>
+      <c r="B9" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="33" t="s">
+        <v>46</v>
+      </c>
+      <c r="D9" s="38" t="s">
+        <v>47</v>
+      </c>
+      <c r="E9" s="32" t="s">
+        <v>41</v>
+      </c>
+      <c r="F9" s="35" t="s">
+        <v>42</v>
+      </c>
+      <c r="G9" s="35" t="s">
+        <v>43</v>
+      </c>
+      <c r="H9" s="36" t="s">
+        <v>37</v>
+      </c>
+      <c r="I9" s="33" t="s">
+        <v>44</v>
+      </c>
+      <c r="J9" s="40" t="s">
+        <v>45</v>
+      </c>
+      <c r="K9" s="32">
+        <v>1</v>
+      </c>
+      <c r="L9" s="32" t="s">
+        <v>158</v>
+      </c>
+      <c r="M9" s="32">
+        <v>1</v>
+      </c>
+      <c r="N9" s="32" t="s">
+        <v>157</v>
+      </c>
+      <c r="O9" s="32" t="s">
+        <v>155</v>
+      </c>
+      <c r="P9" s="33"/>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A10" s="32">
+        <v>9</v>
+      </c>
+      <c r="B10" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="33" t="s">
+        <v>48</v>
+      </c>
+      <c r="D10" s="38" t="s">
+        <v>49</v>
+      </c>
+      <c r="E10" s="32" t="s">
+        <v>41</v>
+      </c>
+      <c r="F10" s="35" t="s">
+        <v>42</v>
+      </c>
+      <c r="G10" s="35" t="s">
+        <v>43</v>
+      </c>
+      <c r="H10" s="36" t="s">
+        <v>50</v>
+      </c>
+      <c r="I10" s="33" t="s">
+        <v>44</v>
+      </c>
+      <c r="J10" s="40" t="s">
+        <v>45</v>
+      </c>
+      <c r="K10" s="32">
+        <v>3</v>
+      </c>
+      <c r="L10" s="32" t="s">
+        <v>158</v>
+      </c>
+      <c r="M10" s="32">
+        <v>3</v>
+      </c>
+      <c r="N10" s="32" t="s">
+        <v>157</v>
+      </c>
+      <c r="O10" s="32" t="s">
+        <v>51</v>
+      </c>
+      <c r="P10" s="33"/>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A11" s="32">
+        <v>10</v>
+      </c>
+      <c r="B11" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="33" t="s">
+        <v>52</v>
+      </c>
+      <c r="D11" s="38" t="s">
+        <v>53</v>
+      </c>
+      <c r="E11" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11" s="35"/>
+      <c r="G11" s="35"/>
+      <c r="H11" s="36" t="s">
+        <v>18</v>
+      </c>
+      <c r="I11" s="33"/>
+      <c r="J11" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="K11" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="L11" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="M11" s="32">
+        <v>2</v>
+      </c>
+      <c r="N11" s="32" t="s">
+        <v>158</v>
+      </c>
+      <c r="O11" s="37" t="s">
+        <v>21</v>
+      </c>
+      <c r="P11" s="33" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A12" s="32">
         <v>11</v>
       </c>
-      <c r="M1" s="15" t="s">
+      <c r="B12" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" s="33" t="s">
+        <v>54</v>
+      </c>
+      <c r="D12" s="38" t="s">
+        <v>55</v>
+      </c>
+      <c r="E12" s="32" t="s">
+        <v>41</v>
+      </c>
+      <c r="F12" s="35" t="s">
+        <v>42</v>
+      </c>
+      <c r="G12" s="35" t="s">
+        <v>43</v>
+      </c>
+      <c r="H12" s="36" t="s">
+        <v>37</v>
+      </c>
+      <c r="I12" s="33" t="s">
+        <v>56</v>
+      </c>
+      <c r="J12" s="40" t="s">
+        <v>45</v>
+      </c>
+      <c r="K12" s="32">
+        <v>3</v>
+      </c>
+      <c r="L12" s="32" t="s">
+        <v>158</v>
+      </c>
+      <c r="M12" s="32">
+        <v>2</v>
+      </c>
+      <c r="N12" s="32" t="s">
+        <v>157</v>
+      </c>
+      <c r="O12" s="32" t="s">
+        <v>51</v>
+      </c>
+      <c r="P12" s="33"/>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A13" s="32">
         <v>12</v>
       </c>
-      <c r="N1" s="15" t="s">
+      <c r="B13" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="33" t="s">
+        <v>57</v>
+      </c>
+      <c r="D13" s="38" t="s">
+        <v>20</v>
+      </c>
+      <c r="E13" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="F13" s="35"/>
+      <c r="G13" s="35"/>
+      <c r="H13" s="36" t="s">
+        <v>18</v>
+      </c>
+      <c r="I13" s="33" t="s">
+        <v>58</v>
+      </c>
+      <c r="J13" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="K13" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="L13" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="M13" s="32">
+        <v>2</v>
+      </c>
+      <c r="N13" s="32" t="s">
+        <v>158</v>
+      </c>
+      <c r="O13" s="32" t="s">
+        <v>59</v>
+      </c>
+      <c r="P13" s="33" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A14" s="32">
         <v>13</v>
       </c>
-      <c r="O1" s="16"/>
+      <c r="B14" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="33" t="s">
+        <v>61</v>
+      </c>
+      <c r="D14" s="38" t="s">
+        <v>20</v>
+      </c>
+      <c r="E14" s="32" t="s">
+        <v>62</v>
+      </c>
+      <c r="F14" s="35"/>
+      <c r="G14" s="35"/>
+      <c r="H14" s="36" t="s">
+        <v>18</v>
+      </c>
+      <c r="I14" s="33" t="s">
+        <v>63</v>
+      </c>
+      <c r="J14" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="K14" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="L14" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="M14" s="32">
+        <v>2</v>
+      </c>
+      <c r="N14" s="32" t="s">
+        <v>158</v>
+      </c>
+      <c r="O14" s="32" t="s">
+        <v>59</v>
+      </c>
+      <c r="P14" s="33" t="s">
+        <v>64</v>
+      </c>
     </row>
-    <row r="2" spans="1:15">
-      <c r="A2" s="4">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A15" s="32">
+        <v>14</v>
+      </c>
+      <c r="B15" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" s="33" t="s">
+        <v>65</v>
+      </c>
+      <c r="D15" s="38" t="s">
+        <v>66</v>
+      </c>
+      <c r="E15" s="32" t="s">
+        <v>62</v>
+      </c>
+      <c r="F15" s="35" t="s">
+        <v>67</v>
+      </c>
+      <c r="G15" s="35"/>
+      <c r="H15" s="36" t="s">
+        <v>50</v>
+      </c>
+      <c r="I15" s="33" t="s">
+        <v>63</v>
+      </c>
+      <c r="J15" s="41" t="s">
+        <v>45</v>
+      </c>
+      <c r="K15" s="32">
+        <v>10</v>
+      </c>
+      <c r="L15" s="32" t="s">
+        <v>157</v>
+      </c>
+      <c r="M15" s="32">
+        <v>3</v>
+      </c>
+      <c r="N15" s="32" t="s">
+        <v>161</v>
+      </c>
+      <c r="O15" s="32" t="s">
+        <v>51</v>
+      </c>
+      <c r="P15" s="33" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A16" s="32">
+        <v>15</v>
+      </c>
+      <c r="B16" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" s="33" t="s">
+        <v>69</v>
+      </c>
+      <c r="D16" s="38" t="s">
+        <v>20</v>
+      </c>
+      <c r="E16" s="32" t="s">
+        <v>41</v>
+      </c>
+      <c r="F16" s="35"/>
+      <c r="G16" s="35"/>
+      <c r="H16" s="36" t="s">
+        <v>18</v>
+      </c>
+      <c r="I16" s="33" t="s">
+        <v>58</v>
+      </c>
+      <c r="J16" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="K16" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="L16" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="M16" s="32">
+        <v>2</v>
+      </c>
+      <c r="N16" s="32" t="s">
+        <v>158</v>
+      </c>
+      <c r="O16" s="32" t="s">
+        <v>162</v>
+      </c>
+      <c r="P16" s="33" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A17" s="32">
+        <v>16</v>
+      </c>
+      <c r="B17" s="33" t="s">
+        <v>71</v>
+      </c>
+      <c r="C17" s="33" t="s">
+        <v>15</v>
+      </c>
+      <c r="D17" s="38" t="s">
+        <v>72</v>
+      </c>
+      <c r="E17" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="F17" s="35" t="s">
+        <v>73</v>
+      </c>
+      <c r="G17" s="35" t="s">
+        <v>74</v>
+      </c>
+      <c r="H17" s="36" t="s">
+        <v>27</v>
+      </c>
+      <c r="I17" s="33" t="s">
+        <v>75</v>
+      </c>
+      <c r="J17" s="40" t="s">
+        <v>76</v>
+      </c>
+      <c r="K17" s="32">
+        <v>5</v>
+      </c>
+      <c r="L17" s="32" t="s">
+        <v>158</v>
+      </c>
+      <c r="M17" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="N17" s="32" t="s">
+        <v>159</v>
+      </c>
+      <c r="O17" s="32" t="s">
+        <v>77</v>
+      </c>
+      <c r="P17" s="33"/>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A18" s="32">
+        <v>17</v>
+      </c>
+      <c r="B18" s="33" t="s">
+        <v>71</v>
+      </c>
+      <c r="C18" s="33" t="s">
+        <v>78</v>
+      </c>
+      <c r="D18" s="34" t="s">
+        <v>79</v>
+      </c>
+      <c r="E18" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="F18" s="35" t="s">
+        <v>80</v>
+      </c>
+      <c r="G18" s="35" t="s">
+        <v>81</v>
+      </c>
+      <c r="H18" s="36" t="s">
+        <v>27</v>
+      </c>
+      <c r="I18" s="33" t="s">
+        <v>82</v>
+      </c>
+      <c r="J18" s="40" t="s">
+        <v>83</v>
+      </c>
+      <c r="K18" s="32">
+        <v>2</v>
+      </c>
+      <c r="L18" s="32" t="s">
+        <v>158</v>
+      </c>
+      <c r="M18" s="32">
+        <v>2</v>
+      </c>
+      <c r="N18" s="32" t="s">
+        <v>159</v>
+      </c>
+      <c r="O18" s="32" t="s">
+        <v>77</v>
+      </c>
+      <c r="P18" s="33"/>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A19" s="32">
+        <v>18</v>
+      </c>
+      <c r="B19" s="33" t="s">
+        <v>71</v>
+      </c>
+      <c r="C19" s="33" t="s">
+        <v>84</v>
+      </c>
+      <c r="D19" s="38" t="s">
+        <v>85</v>
+      </c>
+      <c r="E19" s="32" t="s">
+        <v>41</v>
+      </c>
+      <c r="F19" s="35" t="s">
+        <v>80</v>
+      </c>
+      <c r="G19" s="35" t="s">
+        <v>81</v>
+      </c>
+      <c r="H19" s="36" t="s">
+        <v>27</v>
+      </c>
+      <c r="I19" s="33" t="s">
+        <v>82</v>
+      </c>
+      <c r="J19" s="40" t="s">
+        <v>83</v>
+      </c>
+      <c r="K19" s="32">
+        <v>2</v>
+      </c>
+      <c r="L19" s="32" t="s">
+        <v>158</v>
+      </c>
+      <c r="M19" s="32">
+        <v>2</v>
+      </c>
+      <c r="N19" s="32" t="s">
+        <v>159</v>
+      </c>
+      <c r="O19" s="32" t="s">
+        <v>77</v>
+      </c>
+      <c r="P19" s="33"/>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A20" s="32">
+        <v>19</v>
+      </c>
+      <c r="B20" s="33" t="s">
+        <v>71</v>
+      </c>
+      <c r="C20" s="33" t="s">
+        <v>86</v>
+      </c>
+      <c r="D20" s="38" t="s">
+        <v>87</v>
+      </c>
+      <c r="E20" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="F20" s="33" t="s">
+        <v>88</v>
+      </c>
+      <c r="G20" s="33"/>
+      <c r="H20" s="36" t="s">
+        <v>50</v>
+      </c>
+      <c r="I20" s="33" t="s">
+        <v>89</v>
+      </c>
+      <c r="J20" s="39" t="s">
+        <v>90</v>
+      </c>
+      <c r="K20" s="32">
+        <v>8</v>
+      </c>
+      <c r="L20" s="32" t="s">
+        <v>157</v>
+      </c>
+      <c r="M20" s="32">
+        <v>2</v>
+      </c>
+      <c r="N20" s="32" t="s">
+        <v>159</v>
+      </c>
+      <c r="O20" s="32" t="s">
+        <v>91</v>
+      </c>
+      <c r="P20" s="33"/>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A21" s="32">
+        <v>20</v>
+      </c>
+      <c r="B21" s="33" t="s">
+        <v>71</v>
+      </c>
+      <c r="C21" s="33" t="s">
+        <v>92</v>
+      </c>
+      <c r="D21" s="38" t="s">
+        <v>93</v>
+      </c>
+      <c r="E21" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="F21" s="35" t="s">
+        <v>80</v>
+      </c>
+      <c r="G21" s="35" t="s">
+        <v>81</v>
+      </c>
+      <c r="H21" s="36" t="s">
+        <v>37</v>
+      </c>
+      <c r="I21" s="33" t="s">
+        <v>82</v>
+      </c>
+      <c r="J21" s="40" t="s">
+        <v>83</v>
+      </c>
+      <c r="K21" s="32">
+        <v>4</v>
+      </c>
+      <c r="L21" s="32" t="s">
+        <v>157</v>
+      </c>
+      <c r="M21" s="32">
+        <v>2</v>
+      </c>
+      <c r="N21" s="32" t="s">
+        <v>159</v>
+      </c>
+      <c r="O21" s="32" t="s">
+        <v>77</v>
+      </c>
+      <c r="P21" s="33"/>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A22" s="32">
+        <v>21</v>
+      </c>
+      <c r="B22" s="33" t="s">
+        <v>71</v>
+      </c>
+      <c r="C22" s="33" t="s">
+        <v>94</v>
+      </c>
+      <c r="D22" s="38" t="s">
+        <v>95</v>
+      </c>
+      <c r="E22" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="F22" s="35" t="s">
+        <v>80</v>
+      </c>
+      <c r="G22" s="35" t="s">
+        <v>81</v>
+      </c>
+      <c r="H22" s="36" t="s">
+        <v>37</v>
+      </c>
+      <c r="I22" s="33" t="s">
+        <v>82</v>
+      </c>
+      <c r="J22" s="40" t="s">
+        <v>83</v>
+      </c>
+      <c r="K22" s="32">
+        <v>4</v>
+      </c>
+      <c r="L22" s="32" t="s">
+        <v>157</v>
+      </c>
+      <c r="M22" s="32">
+        <v>2</v>
+      </c>
+      <c r="N22" s="32" t="s">
+        <v>159</v>
+      </c>
+      <c r="O22" s="32" t="s">
+        <v>77</v>
+      </c>
+      <c r="P22" s="33"/>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A23" s="32">
+        <v>22</v>
+      </c>
+      <c r="B23" s="33" t="s">
+        <v>71</v>
+      </c>
+      <c r="C23" s="33" t="s">
+        <v>96</v>
+      </c>
+      <c r="D23" s="38" t="s">
+        <v>97</v>
+      </c>
+      <c r="E23" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="F23" s="35" t="s">
+        <v>98</v>
+      </c>
+      <c r="G23" s="35" t="s">
+        <v>81</v>
+      </c>
+      <c r="H23" s="36" t="s">
+        <v>37</v>
+      </c>
+      <c r="I23" s="33" t="s">
+        <v>75</v>
+      </c>
+      <c r="J23" s="39" t="s">
+        <v>90</v>
+      </c>
+      <c r="K23" s="32">
+        <v>2</v>
+      </c>
+      <c r="L23" s="32" t="s">
+        <v>157</v>
+      </c>
+      <c r="M23" s="32">
+        <v>2</v>
+      </c>
+      <c r="N23" s="32" t="s">
+        <v>159</v>
+      </c>
+      <c r="O23" s="32" t="s">
+        <v>91</v>
+      </c>
+      <c r="P23" s="33"/>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A24" s="32">
+        <v>23</v>
+      </c>
+      <c r="B24" s="33" t="s">
+        <v>71</v>
+      </c>
+      <c r="C24" s="33" t="s">
+        <v>99</v>
+      </c>
+      <c r="D24" s="34" t="s">
+        <v>100</v>
+      </c>
+      <c r="E24" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="F24" s="33" t="s">
+        <v>101</v>
+      </c>
+      <c r="G24" s="35" t="s">
+        <v>81</v>
+      </c>
+      <c r="H24" s="36" t="s">
+        <v>37</v>
+      </c>
+      <c r="I24" s="33" t="s">
+        <v>75</v>
+      </c>
+      <c r="J24" s="39" t="s">
+        <v>90</v>
+      </c>
+      <c r="K24" s="32">
+        <v>2</v>
+      </c>
+      <c r="L24" s="32" t="s">
+        <v>157</v>
+      </c>
+      <c r="M24" s="32">
+        <v>2</v>
+      </c>
+      <c r="N24" s="32" t="s">
+        <v>159</v>
+      </c>
+      <c r="O24" s="32" t="s">
+        <v>77</v>
+      </c>
+      <c r="P24" s="33"/>
+    </row>
+    <row r="25" spans="1:16" ht="21" x14ac:dyDescent="0.3">
+      <c r="A25" s="32">
+        <v>24</v>
+      </c>
+      <c r="B25" s="33" t="s">
+        <v>102</v>
+      </c>
+      <c r="C25" s="33" t="s">
+        <v>103</v>
+      </c>
+      <c r="D25" s="38" t="s">
+        <v>104</v>
+      </c>
+      <c r="E25" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="F25" s="35" t="s">
+        <v>105</v>
+      </c>
+      <c r="G25" s="35" t="s">
+        <v>43</v>
+      </c>
+      <c r="H25" s="36" t="s">
+        <v>27</v>
+      </c>
+      <c r="I25" s="42" t="s">
+        <v>106</v>
+      </c>
+      <c r="J25" s="40" t="s">
+        <v>45</v>
+      </c>
+      <c r="K25" s="32">
+        <v>2</v>
+      </c>
+      <c r="L25" s="32" t="s">
+        <v>158</v>
+      </c>
+      <c r="M25" s="32">
+        <v>2</v>
+      </c>
+      <c r="N25" s="32" t="s">
+        <v>157</v>
+      </c>
+      <c r="O25" s="32" t="s">
+        <v>107</v>
+      </c>
+      <c r="P25" s="43" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" ht="52.5" x14ac:dyDescent="0.3">
+      <c r="A26" s="32">
+        <v>25</v>
+      </c>
+      <c r="B26" s="33" t="s">
+        <v>102</v>
+      </c>
+      <c r="C26" s="33" t="s">
+        <v>109</v>
+      </c>
+      <c r="D26" s="38" t="s">
+        <v>110</v>
+      </c>
+      <c r="E26" s="32" t="s">
+        <v>62</v>
+      </c>
+      <c r="F26" s="35" t="s">
+        <v>111</v>
+      </c>
+      <c r="G26" s="42" t="s">
+        <v>112</v>
+      </c>
+      <c r="H26" s="36" t="s">
+        <v>37</v>
+      </c>
+      <c r="I26" s="33" t="s">
+        <v>113</v>
+      </c>
+      <c r="J26" s="40" t="s">
+        <v>45</v>
+      </c>
+      <c r="K26" s="32">
+        <v>7</v>
+      </c>
+      <c r="L26" s="32" t="s">
+        <v>157</v>
+      </c>
+      <c r="M26" s="32">
+        <v>4</v>
+      </c>
+      <c r="N26" s="32" t="s">
+        <v>161</v>
+      </c>
+      <c r="O26" s="32" t="s">
+        <v>107</v>
+      </c>
+      <c r="P26" s="44" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" ht="52.5" x14ac:dyDescent="0.3">
+      <c r="A27" s="32">
+        <v>26</v>
+      </c>
+      <c r="B27" s="33" t="s">
+        <v>102</v>
+      </c>
+      <c r="C27" s="33" t="s">
+        <v>86</v>
+      </c>
+      <c r="D27" s="38" t="s">
+        <v>115</v>
+      </c>
+      <c r="E27" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="F27" s="33" t="s">
+        <v>88</v>
+      </c>
+      <c r="G27" s="33"/>
+      <c r="H27" s="36" t="s">
+        <v>50</v>
+      </c>
+      <c r="I27" s="33" t="s">
+        <v>89</v>
+      </c>
+      <c r="J27" s="39" t="s">
+        <v>90</v>
+      </c>
+      <c r="K27" s="32">
+        <v>9</v>
+      </c>
+      <c r="L27" s="32" t="s">
+        <v>157</v>
+      </c>
+      <c r="M27" s="32">
+        <v>2</v>
+      </c>
+      <c r="N27" s="32" t="s">
+        <v>161</v>
+      </c>
+      <c r="O27" s="32" t="s">
+        <v>116</v>
+      </c>
+      <c r="P27" s="44" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A28" s="32">
+        <v>27</v>
+      </c>
+      <c r="B28" s="33" t="s">
+        <v>102</v>
+      </c>
+      <c r="C28" s="33" t="s">
+        <v>118</v>
+      </c>
+      <c r="D28" s="38" t="s">
+        <v>119</v>
+      </c>
+      <c r="E28" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="F28" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="G28" s="35"/>
+      <c r="H28" s="36" t="s">
+        <v>37</v>
+      </c>
+      <c r="I28" s="33" t="s">
+        <v>28</v>
+      </c>
+      <c r="J28" s="39" t="s">
+        <v>29</v>
+      </c>
+      <c r="K28" s="32">
         <v>1</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="L28" s="32" t="s">
+        <v>157</v>
+      </c>
+      <c r="M28" s="32">
+        <v>1</v>
+      </c>
+      <c r="N28" s="32" t="s">
+        <v>161</v>
+      </c>
+      <c r="O28" s="32" t="s">
+        <v>107</v>
+      </c>
+      <c r="P28" s="44" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" ht="31.5" x14ac:dyDescent="0.3">
+      <c r="A29" s="32">
+        <v>28</v>
+      </c>
+      <c r="B29" s="33" t="s">
+        <v>102</v>
+      </c>
+      <c r="C29" s="33" t="s">
+        <v>54</v>
+      </c>
+      <c r="D29" s="38" t="s">
+        <v>121</v>
+      </c>
+      <c r="E29" s="32" t="s">
+        <v>41</v>
+      </c>
+      <c r="F29" s="33" t="s">
+        <v>42</v>
+      </c>
+      <c r="G29" s="35" t="s">
+        <v>43</v>
+      </c>
+      <c r="H29" s="36" t="s">
+        <v>27</v>
+      </c>
+      <c r="I29" s="44" t="s">
+        <v>122</v>
+      </c>
+      <c r="J29" s="40" t="s">
+        <v>45</v>
+      </c>
+      <c r="K29" s="32">
+        <v>3</v>
+      </c>
+      <c r="L29" s="32" t="s">
+        <v>158</v>
+      </c>
+      <c r="M29" s="32">
+        <v>1</v>
+      </c>
+      <c r="N29" s="32" t="s">
+        <v>157</v>
+      </c>
+      <c r="O29" s="32" t="s">
+        <v>116</v>
+      </c>
+      <c r="P29" s="43" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A30" s="32">
+        <v>29</v>
+      </c>
+      <c r="B30" s="33" t="s">
+        <v>124</v>
+      </c>
+      <c r="C30" s="33" t="s">
+        <v>125</v>
+      </c>
+      <c r="D30" s="38" t="s">
+        <v>126</v>
+      </c>
+      <c r="E30" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="F30" s="35" t="s">
+        <v>127</v>
+      </c>
+      <c r="G30" s="35"/>
+      <c r="H30" s="36" t="s">
+        <v>50</v>
+      </c>
+      <c r="I30" s="35" t="s">
+        <v>128</v>
+      </c>
+      <c r="J30" s="41"/>
+      <c r="K30" s="32" t="s">
+        <v>129</v>
+      </c>
+      <c r="L30" s="32"/>
+      <c r="M30" s="32">
+        <v>1</v>
+      </c>
+      <c r="N30" s="32"/>
+      <c r="O30" s="32"/>
+      <c r="P30" s="33" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A31" s="32">
+        <v>30</v>
+      </c>
+      <c r="B31" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" s="42" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" s="4" t="s">
+      <c r="C31" s="33" t="s">
+        <v>131</v>
+      </c>
+      <c r="D31" s="38" t="s">
+        <v>132</v>
+      </c>
+      <c r="E31" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="J2" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="K2" s="8">
-        <v>0.5</v>
-      </c>
-      <c r="L2" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="N2" s="9" t="s">
-        <v>22</v>
+      <c r="F31" s="35" t="s">
+        <v>88</v>
+      </c>
+      <c r="G31" s="35"/>
+      <c r="H31" s="36" t="s">
+        <v>50</v>
+      </c>
+      <c r="I31" s="33" t="s">
+        <v>89</v>
+      </c>
+      <c r="J31" s="39" t="s">
+        <v>133</v>
+      </c>
+      <c r="K31" s="32">
+        <v>4</v>
+      </c>
+      <c r="L31" s="32" t="s">
+        <v>157</v>
+      </c>
+      <c r="M31" s="32">
+        <v>1</v>
+      </c>
+      <c r="N31" s="32" t="s">
+        <v>161</v>
+      </c>
+      <c r="O31" s="32" t="s">
+        <v>155</v>
+      </c>
+      <c r="P31" s="33" t="s">
+        <v>134</v>
       </c>
     </row>
-    <row r="3" spans="1:15">
-      <c r="A3" s="4">
-        <v>2</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D3" s="43" t="s">
-        <v>20</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="I3" s="9"/>
-      <c r="J3" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="K3" s="8">
-        <v>3</v>
-      </c>
-      <c r="L3" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="M3" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="N3" s="9" t="s">
-        <v>22</v>
+    <row r="32" spans="1:16" ht="29.15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="32">
+        <v>31</v>
+      </c>
+      <c r="B32" s="33" t="s">
+        <v>102</v>
+      </c>
+      <c r="C32" s="33" t="s">
+        <v>135</v>
+      </c>
+      <c r="D32" s="38" t="s">
+        <v>136</v>
+      </c>
+      <c r="E32" s="32" t="s">
+        <v>41</v>
+      </c>
+      <c r="F32" s="35" t="s">
+        <v>127</v>
+      </c>
+      <c r="G32" s="33"/>
+      <c r="H32" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="I32" s="35" t="s">
+        <v>128</v>
+      </c>
+      <c r="J32" s="41" t="s">
+        <v>137</v>
+      </c>
+      <c r="K32" s="32">
+        <v>25</v>
+      </c>
+      <c r="L32" s="32" t="s">
+        <v>159</v>
+      </c>
+      <c r="M32" s="32">
+        <v>4</v>
+      </c>
+      <c r="N32" s="32"/>
+      <c r="O32" s="45"/>
+      <c r="P32" s="33" t="s">
+        <v>68</v>
       </c>
     </row>
-    <row r="4" spans="1:15">
-      <c r="A4" s="4">
-        <v>3</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D4" s="42" t="s">
-        <v>25</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="G4" s="6"/>
-      <c r="H4" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="I4" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="J4" s="19" t="s">
-        <v>29</v>
-      </c>
-      <c r="K4" s="8">
-        <v>2</v>
-      </c>
-      <c r="L4" s="8">
-        <v>2</v>
-      </c>
-      <c r="M4" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="N4" s="9"/>
-    </row>
-    <row r="5" spans="1:15">
-      <c r="A5" s="4">
-        <v>4</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D5" s="42" t="s">
-        <v>32</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="I5" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="J5" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="K5" s="8">
-        <v>3</v>
-      </c>
-      <c r="L5" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="M5" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="N5" s="9" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15">
-      <c r="A6" s="4">
-        <v>5</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="D6" s="43" t="s">
-        <v>20</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="I6" s="9"/>
-      <c r="J6" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="K6" s="8">
-        <v>2</v>
-      </c>
-      <c r="L6" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="M6" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="N6" s="9" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15">
-      <c r="A7" s="4">
-        <v>6</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="D7" s="43" t="s">
-        <v>36</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F7" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="G7" s="6"/>
-      <c r="H7" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="I7" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="J7" s="18" t="s">
-        <v>29</v>
-      </c>
-      <c r="K7" s="8">
-        <v>2</v>
-      </c>
-      <c r="L7" s="8">
-        <v>3</v>
-      </c>
-      <c r="M7" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="N7" s="9" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15">
-      <c r="A8" s="4">
-        <v>7</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="D8" s="43" t="s">
-        <v>41</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="F8" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="G8" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="H8" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="I8" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="J8" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="K8" s="8">
-        <v>1</v>
-      </c>
-      <c r="L8" s="8">
-        <v>3</v>
-      </c>
-      <c r="M8" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="N8" s="9"/>
-    </row>
-    <row r="9" spans="1:15">
-      <c r="A9" s="4">
-        <v>8</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="D9" s="43" t="s">
-        <v>48</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="G9" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="H9" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="I9" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="J9" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="K9" s="8">
-        <v>1</v>
-      </c>
-      <c r="L9" s="8">
-        <v>1</v>
-      </c>
-      <c r="M9" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="N9" s="9"/>
-    </row>
-    <row r="10" spans="1:15">
-      <c r="A10" s="4">
-        <v>9</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="D10" s="43" t="s">
-        <v>50</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="F10" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="G10" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="H10" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="I10" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="J10" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="K10" s="8">
-        <v>3</v>
-      </c>
-      <c r="L10" s="8">
-        <v>3</v>
-      </c>
-      <c r="M10" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="N10" s="9"/>
-    </row>
-    <row r="11" spans="1:15">
-      <c r="A11" s="4">
-        <v>10</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="D11" s="43" t="s">
-        <v>54</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="I11" s="9"/>
-      <c r="J11" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="K11" s="8">
-        <v>2</v>
-      </c>
-      <c r="L11" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="M11" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="N11" s="9" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15">
-      <c r="A12" s="4">
-        <v>11</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="D12" s="43" t="s">
-        <v>56</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="F12" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="G12" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="H12" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="I12" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="J12" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="K12" s="8">
-        <v>2</v>
-      </c>
-      <c r="L12" s="8">
-        <v>3</v>
-      </c>
-      <c r="M12" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="N12" s="9"/>
-    </row>
-    <row r="13" spans="1:15">
-      <c r="A13" s="4">
-        <v>12</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="D13" s="43" t="s">
-        <v>20</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="I13" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="J13" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="K13" s="8">
-        <v>2</v>
-      </c>
-      <c r="L13" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="M13" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="N13" s="9" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15">
-      <c r="A14" s="4">
-        <v>13</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="D14" s="43" t="s">
-        <v>20</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="I14" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="J14" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="K14" s="8">
-        <v>2</v>
-      </c>
-      <c r="L14" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="M14" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="N14" s="9" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15">
-      <c r="A15" s="4">
-        <v>14</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="D15" s="43" t="s">
-        <v>67</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="F15" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="G15" s="6"/>
-      <c r="H15" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="I15" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="J15" s="20" t="s">
-        <v>46</v>
-      </c>
-      <c r="K15" s="8">
-        <v>3</v>
-      </c>
-      <c r="L15" s="8">
-        <v>10</v>
-      </c>
-      <c r="M15" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="N15" s="9" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15">
-      <c r="A16" s="4">
-        <v>15</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="D16" s="43" t="s">
-        <v>20</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="F16" s="6"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="I16" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="J16" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="K16" s="8">
-        <v>2</v>
-      </c>
-      <c r="L16" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="M16" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="N16" s="9" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14">
-      <c r="A17" s="4">
-        <v>16</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D17" s="43" t="s">
-        <v>73</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F17" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="G17" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="H17" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="I17" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="J17" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="K17" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="L17" s="8">
-        <v>5</v>
-      </c>
-      <c r="M17" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="N17" s="9"/>
-    </row>
-    <row r="18" spans="1:14">
-      <c r="A18" s="4">
-        <v>17</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="D18" s="42" t="s">
-        <v>80</v>
-      </c>
-      <c r="E18" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F18" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="G18" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="H18" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="I18" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="J18" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="K18" s="8">
-        <v>2</v>
-      </c>
-      <c r="L18" s="8">
-        <v>2</v>
-      </c>
-      <c r="M18" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="N18" s="9"/>
-    </row>
-    <row r="19" spans="1:14">
-      <c r="A19" s="4">
-        <v>18</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="D19" s="43" t="s">
-        <v>86</v>
-      </c>
-      <c r="E19" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="F19" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="G19" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="H19" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="I19" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="J19" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="K19" s="8">
-        <v>2</v>
-      </c>
-      <c r="L19" s="8">
-        <v>2</v>
-      </c>
-      <c r="M19" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="N19" s="9"/>
-    </row>
-    <row r="20" spans="1:14">
-      <c r="A20" s="4">
-        <v>19</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="D20" s="43" t="s">
-        <v>88</v>
-      </c>
-      <c r="E20" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F20" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="G20" s="5"/>
-      <c r="H20" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="I20" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="J20" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="K20" s="8">
-        <v>2</v>
-      </c>
-      <c r="L20" s="8">
-        <v>8</v>
-      </c>
-      <c r="M20" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="N20" s="9"/>
-    </row>
-    <row r="21" spans="1:14">
-      <c r="A21" s="4">
-        <v>20</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="D21" s="43" t="s">
-        <v>94</v>
-      </c>
-      <c r="E21" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F21" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="G21" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="H21" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="I21" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="J21" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="K21" s="8">
-        <v>2</v>
-      </c>
-      <c r="L21" s="8">
-        <v>4</v>
-      </c>
-      <c r="M21" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="N21" s="9"/>
-    </row>
-    <row r="22" spans="1:14">
-      <c r="A22" s="4">
-        <v>21</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="D22" s="43" t="s">
-        <v>96</v>
-      </c>
-      <c r="E22" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F22" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="G22" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="H22" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="I22" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="J22" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="K22" s="8">
-        <v>2</v>
-      </c>
-      <c r="L22" s="8">
-        <v>4</v>
-      </c>
-      <c r="M22" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="N22" s="9"/>
-    </row>
-    <row r="23" spans="1:14">
-      <c r="A23" s="4">
-        <v>22</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="D23" s="43" t="s">
-        <v>98</v>
-      </c>
-      <c r="E23" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F23" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="G23" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="H23" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="I23" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="J23" s="19" t="s">
-        <v>91</v>
-      </c>
-      <c r="K23" s="8">
-        <v>2</v>
-      </c>
-      <c r="L23" s="8">
-        <v>2</v>
-      </c>
-      <c r="M23" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="N23" s="9"/>
-    </row>
-    <row r="24" spans="1:14">
-      <c r="A24" s="4">
-        <v>23</v>
-      </c>
-      <c r="B24" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="D24" s="42" t="s">
-        <v>101</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F24" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="G24" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="H24" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="I24" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="J24" s="19" t="s">
-        <v>91</v>
-      </c>
-      <c r="K24" s="8">
-        <v>2</v>
-      </c>
-      <c r="L24" s="8">
-        <v>2</v>
-      </c>
-      <c r="M24" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="N24" s="9"/>
-    </row>
-    <row r="25" spans="1:14" ht="42">
-      <c r="A25" s="4">
-        <v>24</v>
-      </c>
-      <c r="B25" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="D25" s="43" t="s">
-        <v>105</v>
-      </c>
-      <c r="E25" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F25" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="G25" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="H25" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="I25" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="J25" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="K25" s="8">
-        <v>2</v>
-      </c>
-      <c r="L25" s="8">
-        <v>2</v>
-      </c>
-      <c r="M25" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="N25" s="12" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14" ht="69.95">
-      <c r="A26" s="4">
-        <v>25</v>
-      </c>
-      <c r="B26" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="D26" s="43" t="s">
-        <v>111</v>
-      </c>
-      <c r="E26" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="F26" s="6" t="s">
-        <v>112</v>
-      </c>
-      <c r="G26" s="11" t="s">
-        <v>113</v>
-      </c>
-      <c r="H26" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="I26" s="9" t="s">
-        <v>114</v>
-      </c>
-      <c r="J26" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="K26" s="8">
-        <v>4</v>
-      </c>
-      <c r="L26" s="8">
-        <v>7</v>
-      </c>
-      <c r="M26" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="N26" s="13" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14" ht="69.95">
-      <c r="A27" s="4">
-        <v>26</v>
-      </c>
-      <c r="B27" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="C27" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="D27" s="43" t="s">
-        <v>116</v>
-      </c>
-      <c r="E27" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F27" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="G27" s="5"/>
-      <c r="H27" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="I27" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="J27" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="K27" s="8">
-        <v>2</v>
-      </c>
-      <c r="L27" s="8">
-        <v>9</v>
-      </c>
-      <c r="M27" s="8" t="s">
-        <v>117</v>
-      </c>
-      <c r="N27" s="13" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="28" spans="1:14" ht="27.95">
-      <c r="A28" s="4">
-        <v>27</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="D28" s="43" t="s">
-        <v>120</v>
-      </c>
-      <c r="E28" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F28" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="G28" s="6"/>
-      <c r="H28" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="I28" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="J28" s="18" t="s">
-        <v>29</v>
-      </c>
-      <c r="K28" s="8">
-        <v>1</v>
-      </c>
-      <c r="L28" s="8">
-        <v>1</v>
-      </c>
-      <c r="M28" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="N28" s="13" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="29" spans="1:14" ht="56.1">
-      <c r="A29" s="8">
-        <v>28</v>
-      </c>
-      <c r="B29" s="9" t="s">
-        <v>103</v>
-      </c>
-      <c r="C29" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="E29" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="F29" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="G29" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="H29" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="I29" s="13" t="s">
-        <v>123</v>
-      </c>
-      <c r="J29" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="K29" s="8">
-        <v>1</v>
-      </c>
-      <c r="L29" s="8">
-        <v>3</v>
-      </c>
-      <c r="M29" s="8" t="s">
-        <v>117</v>
-      </c>
-      <c r="N29" s="12" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="30" spans="1:14">
-      <c r="A30" s="4">
-        <v>29</v>
-      </c>
-      <c r="B30" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="C30" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="D30" s="43" t="s">
-        <v>127</v>
-      </c>
-      <c r="E30" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F30" s="6" t="s">
-        <v>128</v>
-      </c>
-      <c r="G30" s="6"/>
-      <c r="H30" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="I30" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="J30" s="21"/>
-      <c r="K30" s="8">
-        <v>1</v>
-      </c>
-      <c r="L30" s="8" t="s">
-        <v>130</v>
-      </c>
-      <c r="M30" s="8"/>
-      <c r="N30" s="9" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="31" spans="1:14">
-      <c r="A31" s="8">
-        <v>30</v>
-      </c>
-      <c r="B31" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="C31" s="9" t="s">
-        <v>132</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="E31" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="F31" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="G31" s="6"/>
-      <c r="H31" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="I31" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="J31" s="18" t="s">
-        <v>134</v>
-      </c>
-      <c r="K31" s="8">
-        <v>1</v>
-      </c>
-      <c r="L31" s="8">
-        <v>4</v>
-      </c>
-      <c r="M31" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="N31" s="9" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="32" spans="1:14" ht="29.1" customHeight="1">
-      <c r="A32" s="8">
-        <v>31</v>
-      </c>
-      <c r="B32" s="9" t="s">
-        <v>103</v>
-      </c>
-      <c r="C32" s="9" t="s">
-        <v>136</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="E32" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="F32" s="6" t="s">
-        <v>128</v>
-      </c>
-      <c r="G32" s="9"/>
-      <c r="H32" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="I32" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="J32" s="21" t="s">
-        <v>138</v>
-      </c>
-      <c r="K32" s="8">
-        <v>4</v>
-      </c>
-      <c r="L32" s="8">
-        <v>25</v>
-      </c>
-      <c r="M32" s="17" t="s">
-        <v>139</v>
-      </c>
-      <c r="N32" s="9" t="s">
-        <v>69</v>
-      </c>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A33" s="28"/>
+      <c r="B33" s="28"/>
+      <c r="C33" s="28"/>
+      <c r="D33" s="28"/>
+      <c r="E33" s="28"/>
+      <c r="F33" s="28"/>
+      <c r="G33" s="28"/>
+      <c r="I33" s="28"/>
+      <c r="J33" s="29"/>
+      <c r="K33" s="29"/>
+      <c r="L33" s="29"/>
+      <c r="M33" s="29"/>
+      <c r="N33" s="29"/>
+      <c r="O33" s="29"/>
+      <c r="P33" s="28"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:N32"/>
-  <conditionalFormatting sqref="F1:J1 F23 F28:G28 F7:G7 F11:G11 F17:G17 F4:G4 F13:G13 E1:E1048576 F3 F5 F25:F26 F30:G30 F29">
-    <cfRule type="containsText" dxfId="133" priority="137" operator="containsText" text="Low">
+  <autoFilter ref="A1:P32"/>
+  <conditionalFormatting sqref="F23 F28:G28 F7:G7 F11:G11 F17:G17 F4:G4 F13:G13 E1:E1048576 F3 F5 F25:F26 F30:G30 F29 O1 F1:K1">
+    <cfRule type="containsText" dxfId="136" priority="143" operator="containsText" text="Low">
       <formula>NOT(ISERROR(SEARCH("Low",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="132" priority="138" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="135" priority="144" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="131" priority="139" operator="containsText" text="High">
+    <cfRule type="containsText" dxfId="134" priority="145" operator="containsText" text="High">
       <formula>NOT(ISERROR(SEARCH("High",E1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:G2">
-    <cfRule type="containsText" dxfId="130" priority="107" operator="containsText" text="Low">
+    <cfRule type="containsText" dxfId="133" priority="113" operator="containsText" text="Low">
       <formula>NOT(ISERROR(SEARCH("Low",F2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="129" priority="108" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="132" priority="114" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",F2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="128" priority="109" operator="containsText" text="High">
+    <cfRule type="containsText" dxfId="131" priority="115" operator="containsText" text="High">
       <formula>NOT(ISERROR(SEARCH("High",F2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F19">
-    <cfRule type="containsText" dxfId="127" priority="131" operator="containsText" text="Low">
+    <cfRule type="containsText" dxfId="130" priority="137" operator="containsText" text="Low">
       <formula>NOT(ISERROR(SEARCH("Low",F19)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="126" priority="132" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="129" priority="138" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",F19)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="125" priority="133" operator="containsText" text="High">
+    <cfRule type="containsText" dxfId="128" priority="139" operator="containsText" text="High">
       <formula>NOT(ISERROR(SEARCH("High",F19)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F18">
-    <cfRule type="containsText" dxfId="124" priority="128" operator="containsText" text="Low">
+    <cfRule type="containsText" dxfId="127" priority="134" operator="containsText" text="Low">
       <formula>NOT(ISERROR(SEARCH("Low",F18)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="123" priority="129" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="126" priority="135" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",F18)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="122" priority="130" operator="containsText" text="High">
+    <cfRule type="containsText" dxfId="125" priority="136" operator="containsText" text="High">
       <formula>NOT(ISERROR(SEARCH("High",F18)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F6">
-    <cfRule type="containsText" dxfId="121" priority="125" operator="containsText" text="Low">
+    <cfRule type="containsText" dxfId="124" priority="131" operator="containsText" text="Low">
       <formula>NOT(ISERROR(SEARCH("Low",F6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="120" priority="126" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="123" priority="132" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",F6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="119" priority="127" operator="containsText" text="High">
+    <cfRule type="containsText" dxfId="122" priority="133" operator="containsText" text="High">
       <formula>NOT(ISERROR(SEARCH("High",F6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F8:G8">
-    <cfRule type="containsText" dxfId="118" priority="122" operator="containsText" text="Low">
+    <cfRule type="containsText" dxfId="121" priority="128" operator="containsText" text="Low">
       <formula>NOT(ISERROR(SEARCH("Low",F8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="117" priority="123" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="120" priority="129" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",F8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="116" priority="124" operator="containsText" text="High">
+    <cfRule type="containsText" dxfId="119" priority="130" operator="containsText" text="High">
       <formula>NOT(ISERROR(SEARCH("High",F8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F9">
-    <cfRule type="containsText" dxfId="115" priority="119" operator="containsText" text="Low">
+    <cfRule type="containsText" dxfId="118" priority="125" operator="containsText" text="Low">
       <formula>NOT(ISERROR(SEARCH("Low",F9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="114" priority="120" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="117" priority="126" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",F9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="113" priority="121" operator="containsText" text="High">
+    <cfRule type="containsText" dxfId="116" priority="127" operator="containsText" text="High">
       <formula>NOT(ISERROR(SEARCH("High",F9)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F10">
-    <cfRule type="containsText" dxfId="112" priority="116" operator="containsText" text="Low">
+    <cfRule type="containsText" dxfId="115" priority="122" operator="containsText" text="Low">
       <formula>NOT(ISERROR(SEARCH("Low",F10)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="111" priority="117" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="114" priority="123" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",F10)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="110" priority="118" operator="containsText" text="High">
+    <cfRule type="containsText" dxfId="113" priority="124" operator="containsText" text="High">
       <formula>NOT(ISERROR(SEARCH("High",F10)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F12:G12">
-    <cfRule type="containsText" dxfId="109" priority="113" operator="containsText" text="Low">
+    <cfRule type="containsText" dxfId="112" priority="119" operator="containsText" text="Low">
       <formula>NOT(ISERROR(SEARCH("Low",F12)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="108" priority="114" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="111" priority="120" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",F12)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="107" priority="115" operator="containsText" text="High">
+    <cfRule type="containsText" dxfId="110" priority="121" operator="containsText" text="High">
       <formula>NOT(ISERROR(SEARCH("High",F12)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F14:G14">
-    <cfRule type="containsText" dxfId="106" priority="104" operator="containsText" text="Low">
+    <cfRule type="containsText" dxfId="109" priority="110" operator="containsText" text="Low">
       <formula>NOT(ISERROR(SEARCH("Low",F14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="105" priority="105" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="108" priority="111" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",F14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="104" priority="106" operator="containsText" text="High">
+    <cfRule type="containsText" dxfId="107" priority="112" operator="containsText" text="High">
       <formula>NOT(ISERROR(SEARCH("High",F14)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F15:G15">
-    <cfRule type="containsText" dxfId="103" priority="101" operator="containsText" text="Low">
+    <cfRule type="containsText" dxfId="106" priority="107" operator="containsText" text="Low">
       <formula>NOT(ISERROR(SEARCH("Low",F15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="102" priority="102" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="105" priority="108" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",F15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="101" priority="103" operator="containsText" text="High">
+    <cfRule type="containsText" dxfId="104" priority="109" operator="containsText" text="High">
       <formula>NOT(ISERROR(SEARCH("High",F15)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F16:G16">
-    <cfRule type="containsText" dxfId="100" priority="95" operator="containsText" text="Low">
+    <cfRule type="containsText" dxfId="103" priority="101" operator="containsText" text="Low">
       <formula>NOT(ISERROR(SEARCH("Low",F16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="99" priority="96" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="102" priority="102" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",F16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="98" priority="97" operator="containsText" text="High">
+    <cfRule type="containsText" dxfId="101" priority="103" operator="containsText" text="High">
       <formula>NOT(ISERROR(SEARCH("High",F16)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:H1048576">
-    <cfRule type="containsText" dxfId="97" priority="46" operator="containsText" text="Not Developed">
+    <cfRule type="containsText" dxfId="100" priority="52" operator="containsText" text="Not Developed">
       <formula>NOT(ISERROR(SEARCH("Not Developed",H1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="96" priority="92" operator="containsText" text="Not Yet Integrated">
+    <cfRule type="containsText" dxfId="99" priority="98" operator="containsText" text="Not Yet Integrated">
       <formula>NOT(ISERROR(SEARCH("Not Yet Integrated",H1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="95" priority="93" operator="containsText" text="In-Progress">
+    <cfRule type="containsText" dxfId="98" priority="99" operator="containsText" text="In-Progress">
       <formula>NOT(ISERROR(SEARCH("In-Progress",H1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="94" priority="94" operator="containsText" text="Dev Completed">
+    <cfRule type="containsText" dxfId="97" priority="100" operator="containsText" text="Dev Completed">
       <formula>NOT(ISERROR(SEARCH("Dev Completed",H1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K1">
-    <cfRule type="containsText" dxfId="93" priority="89" operator="containsText" text="Low">
-      <formula>NOT(ISERROR(SEARCH("Low",K1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="92" priority="90" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",K1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="91" priority="91" operator="containsText" text="High">
-      <formula>NOT(ISERROR(SEARCH("High",K1)))</formula>
+  <conditionalFormatting sqref="M1">
+    <cfRule type="containsText" dxfId="96" priority="95" operator="containsText" text="Low">
+      <formula>NOT(ISERROR(SEARCH("Low",M1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="95" priority="96" operator="containsText" text="Medium">
+      <formula>NOT(ISERROR(SEARCH("Medium",M1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="94" priority="97" operator="containsText" text="High">
+      <formula>NOT(ISERROR(SEARCH("High",M1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F31:G31">
-    <cfRule type="containsText" dxfId="90" priority="86" operator="containsText" text="Low">
+    <cfRule type="containsText" dxfId="93" priority="92" operator="containsText" text="Low">
       <formula>NOT(ISERROR(SEARCH("Low",F31)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="89" priority="87" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="92" priority="93" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",F31)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="88" priority="88" operator="containsText" text="High">
+    <cfRule type="containsText" dxfId="91" priority="94" operator="containsText" text="High">
       <formula>NOT(ISERROR(SEARCH("High",F31)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G29">
-    <cfRule type="containsText" dxfId="87" priority="47" operator="containsText" text="Low">
+    <cfRule type="containsText" dxfId="90" priority="53" operator="containsText" text="Low">
       <formula>NOT(ISERROR(SEARCH("Low",G29)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="86" priority="48" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="89" priority="54" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",G29)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="85" priority="49" operator="containsText" text="High">
+    <cfRule type="containsText" dxfId="88" priority="55" operator="containsText" text="High">
       <formula>NOT(ISERROR(SEARCH("High",G29)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3">
-    <cfRule type="containsText" dxfId="84" priority="80" operator="containsText" text="Low">
+    <cfRule type="containsText" dxfId="87" priority="86" operator="containsText" text="Low">
       <formula>NOT(ISERROR(SEARCH("Low",G3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="83" priority="81" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="86" priority="87" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",G3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="82" priority="82" operator="containsText" text="High">
+    <cfRule type="containsText" dxfId="85" priority="88" operator="containsText" text="High">
       <formula>NOT(ISERROR(SEARCH("High",G3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G5">
-    <cfRule type="containsText" dxfId="81" priority="77" operator="containsText" text="Low">
+    <cfRule type="containsText" dxfId="84" priority="83" operator="containsText" text="Low">
       <formula>NOT(ISERROR(SEARCH("Low",G5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="80" priority="78" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="83" priority="84" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",G5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="79" priority="79" operator="containsText" text="High">
+    <cfRule type="containsText" dxfId="82" priority="85" operator="containsText" text="High">
       <formula>NOT(ISERROR(SEARCH("High",G5)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G6">
-    <cfRule type="containsText" dxfId="78" priority="74" operator="containsText" text="Low">
+    <cfRule type="containsText" dxfId="81" priority="80" operator="containsText" text="Low">
       <formula>NOT(ISERROR(SEARCH("Low",G6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="77" priority="75" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="80" priority="81" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",G6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="76" priority="76" operator="containsText" text="High">
+    <cfRule type="containsText" dxfId="79" priority="82" operator="containsText" text="High">
       <formula>NOT(ISERROR(SEARCH("High",G6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G9">
-    <cfRule type="containsText" dxfId="75" priority="71" operator="containsText" text="Low">
+    <cfRule type="containsText" dxfId="78" priority="77" operator="containsText" text="Low">
       <formula>NOT(ISERROR(SEARCH("Low",G9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="74" priority="72" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="77" priority="78" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",G9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="73" priority="73" operator="containsText" text="High">
+    <cfRule type="containsText" dxfId="76" priority="79" operator="containsText" text="High">
       <formula>NOT(ISERROR(SEARCH("High",G9)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G10">
-    <cfRule type="containsText" dxfId="72" priority="68" operator="containsText" text="Low">
+    <cfRule type="containsText" dxfId="75" priority="74" operator="containsText" text="Low">
       <formula>NOT(ISERROR(SEARCH("Low",G10)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="71" priority="69" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="74" priority="75" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",G10)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="70" priority="70" operator="containsText" text="High">
+    <cfRule type="containsText" dxfId="73" priority="76" operator="containsText" text="High">
       <formula>NOT(ISERROR(SEARCH("High",G10)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G18">
-    <cfRule type="containsText" dxfId="69" priority="65" operator="containsText" text="Low">
+    <cfRule type="containsText" dxfId="72" priority="71" operator="containsText" text="Low">
       <formula>NOT(ISERROR(SEARCH("Low",G18)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="68" priority="66" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="71" priority="72" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",G18)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="67" priority="67" operator="containsText" text="High">
+    <cfRule type="containsText" dxfId="70" priority="73" operator="containsText" text="High">
       <formula>NOT(ISERROR(SEARCH("High",G18)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G25">
-    <cfRule type="containsText" dxfId="66" priority="53" operator="containsText" text="Low">
+    <cfRule type="containsText" dxfId="69" priority="59" operator="containsText" text="Low">
       <formula>NOT(ISERROR(SEARCH("Low",G25)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="65" priority="54" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="68" priority="60" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",G25)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="64" priority="55" operator="containsText" text="High">
+    <cfRule type="containsText" dxfId="67" priority="61" operator="containsText" text="High">
       <formula>NOT(ISERROR(SEARCH("High",G25)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G26">
-    <cfRule type="containsText" dxfId="63" priority="50" operator="containsText" text="Low">
+    <cfRule type="containsText" dxfId="66" priority="56" operator="containsText" text="Low">
       <formula>NOT(ISERROR(SEARCH("Low",G26)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="62" priority="51" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="65" priority="57" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",G26)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="61" priority="52" operator="containsText" text="High">
+    <cfRule type="containsText" dxfId="64" priority="58" operator="containsText" text="High">
       <formula>NOT(ISERROR(SEARCH("High",G26)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L1:M1">
-    <cfRule type="containsText" dxfId="60" priority="43" operator="containsText" text="Low">
-      <formula>NOT(ISERROR(SEARCH("Low",L1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="59" priority="44" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",L1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="58" priority="45" operator="containsText" text="High">
-      <formula>NOT(ISERROR(SEARCH("High",L1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F32">
-    <cfRule type="containsText" dxfId="57" priority="40" operator="containsText" text="Low">
+    <cfRule type="containsText" dxfId="63" priority="46" operator="containsText" text="Low">
       <formula>NOT(ISERROR(SEARCH("Low",F32)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="56" priority="41" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="62" priority="47" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",F32)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="55" priority="42" operator="containsText" text="High">
+    <cfRule type="containsText" dxfId="61" priority="48" operator="containsText" text="High">
       <formula>NOT(ISERROR(SEARCH("High",F32)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F21">
-    <cfRule type="containsText" dxfId="54" priority="37" operator="containsText" text="Low">
+    <cfRule type="containsText" dxfId="60" priority="43" operator="containsText" text="Low">
       <formula>NOT(ISERROR(SEARCH("Low",F21)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="53" priority="38" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="59" priority="44" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",F21)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="52" priority="39" operator="containsText" text="High">
+    <cfRule type="containsText" dxfId="58" priority="45" operator="containsText" text="High">
       <formula>NOT(ISERROR(SEARCH("High",F21)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F22">
-    <cfRule type="containsText" dxfId="51" priority="31" operator="containsText" text="Low">
+    <cfRule type="containsText" dxfId="57" priority="37" operator="containsText" text="Low">
       <formula>NOT(ISERROR(SEARCH("Low",F22)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="50" priority="32" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="56" priority="38" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",F22)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="49" priority="33" operator="containsText" text="High">
+    <cfRule type="containsText" dxfId="55" priority="39" operator="containsText" text="High">
       <formula>NOT(ISERROR(SEARCH("High",F22)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G19">
-    <cfRule type="containsText" dxfId="48" priority="28" operator="containsText" text="Low">
+    <cfRule type="containsText" dxfId="54" priority="34" operator="containsText" text="Low">
       <formula>NOT(ISERROR(SEARCH("Low",G19)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="47" priority="29" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="53" priority="35" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",G19)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="46" priority="30" operator="containsText" text="High">
+    <cfRule type="containsText" dxfId="52" priority="36" operator="containsText" text="High">
       <formula>NOT(ISERROR(SEARCH("High",G19)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G21">
-    <cfRule type="containsText" dxfId="45" priority="25" operator="containsText" text="Low">
+    <cfRule type="containsText" dxfId="51" priority="31" operator="containsText" text="Low">
       <formula>NOT(ISERROR(SEARCH("Low",G21)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="44" priority="26" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="50" priority="32" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",G21)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="43" priority="27" operator="containsText" text="High">
+    <cfRule type="containsText" dxfId="49" priority="33" operator="containsText" text="High">
       <formula>NOT(ISERROR(SEARCH("High",G21)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G22">
-    <cfRule type="containsText" dxfId="42" priority="22" operator="containsText" text="Low">
+    <cfRule type="containsText" dxfId="48" priority="28" operator="containsText" text="Low">
       <formula>NOT(ISERROR(SEARCH("Low",G22)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="41" priority="23" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="47" priority="29" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",G22)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="40" priority="24" operator="containsText" text="High">
+    <cfRule type="containsText" dxfId="46" priority="30" operator="containsText" text="High">
       <formula>NOT(ISERROR(SEARCH("High",G22)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G23">
-    <cfRule type="containsText" dxfId="39" priority="10" operator="containsText" text="Low">
+    <cfRule type="containsText" dxfId="45" priority="16" operator="containsText" text="Low">
       <formula>NOT(ISERROR(SEARCH("Low",G23)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="38" priority="11" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="44" priority="17" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",G23)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="37" priority="12" operator="containsText" text="High">
+    <cfRule type="containsText" dxfId="43" priority="18" operator="containsText" text="High">
       <formula>NOT(ISERROR(SEARCH("High",G23)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G24">
+    <cfRule type="containsText" dxfId="42" priority="10" operator="containsText" text="Low">
+      <formula>NOT(ISERROR(SEARCH("Low",G24)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="41" priority="11" operator="containsText" text="Medium">
+      <formula>NOT(ISERROR(SEARCH("Medium",G24)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="40" priority="12" operator="containsText" text="High">
+      <formula>NOT(ISERROR(SEARCH("High",G24)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P1">
+    <cfRule type="containsText" dxfId="39" priority="7" operator="containsText" text="Low">
+      <formula>NOT(ISERROR(SEARCH("Low",P1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="38" priority="8" operator="containsText" text="Medium">
+      <formula>NOT(ISERROR(SEARCH("Medium",P1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="37" priority="9" operator="containsText" text="High">
+      <formula>NOT(ISERROR(SEARCH("High",P1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L1">
     <cfRule type="containsText" dxfId="36" priority="4" operator="containsText" text="Low">
-      <formula>NOT(ISERROR(SEARCH("Low",G24)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Low",L1)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="35" priority="5" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",G24)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Medium",L1)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="34" priority="6" operator="containsText" text="High">
-      <formula>NOT(ISERROR(SEARCH("High",G24)))</formula>
+      <formula>NOT(ISERROR(SEARCH("High",L1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N1">
@@ -3851,7 +4143,7 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3863,60 +4155,60 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.85546875" customWidth="1"/>
-    <col min="3" max="3" width="46.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.5703125" customWidth="1"/>
-    <col min="7" max="7" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.28515625" customWidth="1"/>
-    <col min="9" max="9" width="16.5703125" customWidth="1"/>
-    <col min="12" max="12" width="17.140625" customWidth="1"/>
+    <col min="1" max="1" width="6.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.81640625" customWidth="1"/>
+    <col min="3" max="3" width="46.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.54296875" customWidth="1"/>
+    <col min="7" max="7" width="13.26953125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.26953125" customWidth="1"/>
+    <col min="9" max="9" width="16.54296875" customWidth="1"/>
+    <col min="12" max="12" width="17.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="27.95">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:13" ht="28" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="E1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="F1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="G1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="14" t="s">
-        <v>140</v>
-      </c>
-      <c r="I1" s="15" t="s">
+      <c r="H1" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="I1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="15" t="s">
+      <c r="J1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="K1" s="15" t="s">
+      <c r="K1" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="L1" s="15" t="s">
+      <c r="L1" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="M1" s="15" t="s">
+      <c r="M1" s="5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3924,19 +4216,19 @@
         <v>14</v>
       </c>
       <c r="C2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E2" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="G2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -3944,19 +4236,19 @@
         <v>14</v>
       </c>
       <c r="C3" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E3" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="G3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -3964,196 +4256,196 @@
         <v>14</v>
       </c>
       <c r="C4" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E4" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="G4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C5" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E5" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="G5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C6" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E6" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="G6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:13">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
+        <v>143</v>
+      </c>
+      <c r="C7" t="s">
+        <v>144</v>
+      </c>
+      <c r="D7" t="s">
+        <v>62</v>
+      </c>
+      <c r="E7" t="s">
         <v>145</v>
       </c>
-      <c r="C7" t="s">
-        <v>146</v>
-      </c>
-      <c r="D7" t="s">
-        <v>63</v>
-      </c>
-      <c r="E7" t="s">
-        <v>147</v>
-      </c>
       <c r="G7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:13">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C8" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E8" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="G8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:13">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C9" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E9" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="G9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
-    <row r="10" spans="1:13">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C10" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E10" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="G10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:13">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C11" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E11" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="G11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
-    <row r="12" spans="1:13">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C12" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E12" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="G12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
-    <row r="13" spans="1:13">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C13" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E13" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="G13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -4235,71 +4527,71 @@
   <dimension ref="B2:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B5" sqref="B5:G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.7109375" style="22"/>
-    <col min="2" max="2" width="19.28515625" style="23" customWidth="1"/>
-    <col min="3" max="7" width="16.140625" style="22" customWidth="1"/>
-    <col min="8" max="16384" width="8.7109375" style="22"/>
+    <col min="1" max="1" width="8.7265625" style="7"/>
+    <col min="2" max="2" width="19.26953125" style="8" customWidth="1"/>
+    <col min="3" max="7" width="16.1796875" style="7" customWidth="1"/>
+    <col min="8" max="16384" width="8.7265625" style="7"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" ht="15" thickBot="1"/>
-    <row r="3" spans="2:7" ht="15" thickBot="1">
-      <c r="B3" s="30" t="s">
+    <row r="2" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="3" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B3" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="33" t="s">
+      <c r="C3" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="24" t="s">
-        <v>42</v>
-      </c>
-      <c r="E3" s="25" t="s">
-        <v>63</v>
-      </c>
-      <c r="F3" s="34"/>
-      <c r="G3" s="35"/>
+      <c r="D3" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="F3" s="19"/>
+      <c r="G3" s="20"/>
     </row>
-    <row r="4" spans="2:7" ht="15" thickBot="1">
-      <c r="B4" s="31" t="s">
+    <row r="4" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B4" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="39" t="s">
-        <v>155</v>
-      </c>
-      <c r="D4" s="28" t="s">
+      <c r="C4" s="24" t="s">
+        <v>153</v>
+      </c>
+      <c r="D4" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="29" t="s">
+      <c r="E4" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="F4" s="40" t="s">
-        <v>38</v>
-      </c>
-      <c r="G4" s="41" t="s">
-        <v>51</v>
+      <c r="F4" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="G4" s="26" t="s">
+        <v>50</v>
       </c>
     </row>
-    <row r="5" spans="2:7" ht="16.5" customHeight="1" thickBot="1">
-      <c r="B5" s="32" t="s">
+    <row r="5" spans="2:7" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B5" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="36" t="s">
+      <c r="C5" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="26" t="s">
-        <v>156</v>
-      </c>
-      <c r="E5" s="27" t="s">
-        <v>142</v>
-      </c>
-      <c r="F5" s="37" t="s">
+      <c r="D5" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="F5" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="G5" s="38"/>
+      <c r="G5" s="23"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B3">
@@ -4355,6 +4647,32 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <LikesCount xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <ProjectIGName xmlns="fd9ad297-cc8c-4afc-b828-e13c9647a5fa">Mindtree</ProjectIGName>
+    <Ratings xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <LikedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </LikedBy>
+    <ProjectAccountName xmlns="fd9ad297-cc8c-4afc-b828-e13c9647a5fa">Mindtree</ProjectAccountName>
+    <ProjectName xmlns="fd9ad297-cc8c-4afc-b828-e13c9647a5fa">MOSIP</ProjectName>
+    <RatedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </RatedBy>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -4363,7 +4681,7 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="CTDocLibrary" ma:contentTypeID="0x010100C5D5EC2DEF914E3897774E287F80A8FB00C54CAAC0C88AA446A5AFE942C68BA98B" ma:contentTypeVersion="8" ma:contentTypeDescription="My Content Type" ma:contentTypeScope="" ma:versionID="8509de5a9a506e3b9b1fe93a7c193cee">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="fd9ad297-cc8c-4afc-b828-e13c9647a5fa" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b380538c208c9f76b13ef3dbebc9c2d9" ns1:_="" ns2:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -4570,33 +4888,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <LikesCount xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <ProjectIGName xmlns="fd9ad297-cc8c-4afc-b828-e13c9647a5fa">Mindtree</ProjectIGName>
-    <Ratings xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <LikedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </LikedBy>
-    <ProjectAccountName xmlns="fd9ad297-cc8c-4afc-b828-e13c9647a5fa">Mindtree</ProjectAccountName>
-    <ProjectName xmlns="fd9ad297-cc8c-4afc-b828-e13c9647a5fa">MOSIP</ProjectName>
-    <RatedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </RatedBy>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4CD0E17B-AEEB-4677-A897-891D0AFE351C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="fd9ad297-cc8c-4afc-b828-e13c9647a5fa"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2F3AA23D-8B63-492C-BBC7-698CC026E11F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
@@ -4604,7 +4913,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D2280BBD-A5A1-4222-8C04-A224E167DB8E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4621,21 +4930,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4CD0E17B-AEEB-4677-A897-891D0AFE351C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="fd9ad297-cc8c-4afc-b828-e13c9647a5fa"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>